<commit_message>
load pt 1 of the interested parties data
</commit_message>
<xml_diff>
--- a/data/patents/metadata/PT_Data Dictionary - English only.xlsx
+++ b/data/patents/metadata/PT_Data Dictionary - English only.xlsx
@@ -1,46 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\econ899\data\patents\metadata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8613859A-D2B2-4FF0-8ABA-7980269729B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="PT" sheetId="1" r:id="rId1"/>
-    <sheet name="PT_Road_Map" sheetId="2" r:id="rId2"/>
-    <sheet name="PT_Main" sheetId="3" r:id="rId3"/>
-    <sheet name="PT_Interested_Party" sheetId="5" r:id="rId4"/>
-    <sheet name="PT_Priority_Claim" sheetId="4" r:id="rId5"/>
-    <sheet name="PT_Abstract" sheetId="6" r:id="rId6"/>
-    <sheet name="PT_Disclosure" sheetId="7" r:id="rId7"/>
-    <sheet name="PT_Claim" sheetId="8" r:id="rId8"/>
-    <sheet name="PT_IPC_Classification" sheetId="9" r:id="rId9"/>
+    <sheet r:id="rId1" sheetId="1" name="PT"/>
+    <sheet r:id="rId2" sheetId="2" name="PT_Road_Map"/>
+    <sheet r:id="rId3" sheetId="3" name="PT_Main"/>
+    <sheet r:id="rId4" sheetId="4" name="PT_Interested_Party"/>
+    <sheet r:id="rId5" sheetId="5" name="PT_Priority_Claim"/>
+    <sheet r:id="rId6" sheetId="6" name="PT_Abstract"/>
+    <sheet r:id="rId7" sheetId="7" name="PT_Disclosure"/>
+    <sheet r:id="rId8" sheetId="8" name="PT_Claim"/>
+    <sheet r:id="rId9" sheetId="9" name="PT_IPC_Classification"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3">PT_Interested_Party!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2">PT_Main!$A$1:$C$24</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -700,6 +681,85 @@
   <si>
     <t>Cet élément contient le numéro de séquence qui donne l'ordre du texte de l'abrégé pour le fichier en format csv.
 Ex: 1, 2, 3,….</t>
+  </si>
+  <si>
+    <t>PT_Priority_Claim dictionary - Dictionnaire PT_revendication_de_priorité</t>
+  </si>
+  <si>
+    <t>Foreign Application/Patent Number</t>
+  </si>
+  <si>
+    <t>Numéro du brevet étranger / national</t>
+  </si>
+  <si>
+    <t>Foreign application / patent number is the number of the previously filed application
+Ex: 60/508,112</t>
+  </si>
+  <si>
+    <t>Le numéro du brevet étranger / national est le numéro de la demande déposée antérieurement.
+Ex: 60/508,112</t>
+  </si>
+  <si>
+    <t>Priority Claim Kind Code</t>
+  </si>
+  <si>
+    <t>Code de type de revendications de priorité</t>
+  </si>
+  <si>
+    <t>Priority Claim Kind Code indicates if the previously filed application was filed in Canada or not.
+Ex: INTERNATIONAL, NATIONAL</t>
+  </si>
+  <si>
+    <t>Le code de type de revendications de priorité indique si la demande déposée antérieurement a été effectuée au Canada ou à l'étranger.
+Ex: INTERNATIONAL, NATIONAL</t>
+  </si>
+  <si>
+    <t>Priority Claim Country Code</t>
+  </si>
+  <si>
+    <t>Code du pays d'origine de revendications de priorité</t>
+  </si>
+  <si>
+    <t>Country code of the previously filed application
+Ex: CA, US
+Detail definition (STANDARD ST.3) can be found at:
+https://www.wipo.int/export/sites/www/standards/en/pdf/03-03-01.pdf</t>
+  </si>
+  <si>
+    <t>Le code du pays d'origine d'une demande déposée antérieurement.
+Ex: CA, US
+La définition détaillée (STANDARD ST.3) peut être trouvée à l'adresse suivante:
+https://www.wipo.int/export/sites/www/standards/fr/pdf/03-03-01.pdf</t>
+  </si>
+  <si>
+    <t>Priority Claim Country</t>
+  </si>
+  <si>
+    <t>Pays d'origine de revendications de priorité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country of the the previously filed application
+Ex: Canada, United States of America </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le pays d'origine d'une demande déposée antérieurement
+Ex: Canada, United States of America </t>
+  </si>
+  <si>
+    <t>Priority Claim Calendar Dt</t>
+  </si>
+  <si>
+    <t>Date de revendications de priorité</t>
+  </si>
+  <si>
+    <t>Date of the the previously filed application
+YYYY-MM-DD
+Ex: 2017-02-17</t>
+  </si>
+  <si>
+    <t>La date de dépôt d'une demande antérieure
+AAAA-MM-JJ
+Ex: 2017-02-17</t>
   </si>
   <si>
     <t>Agent Type Code</t>
@@ -845,85 +905,6 @@
   <si>
     <t xml:space="preserve">This element contains the name of the country of the  interested party according to WIPO ST.3, if available.
 Ex: Canada, United States of America </t>
-  </si>
-  <si>
-    <t>PT_Priority_Claim dictionary - Dictionnaire PT_revendication_de_priorité</t>
-  </si>
-  <si>
-    <t>Foreign Application/Patent Number</t>
-  </si>
-  <si>
-    <t>Numéro du brevet étranger / national</t>
-  </si>
-  <si>
-    <t>Foreign application / patent number is the number of the previously filed application
-Ex: 60/508,112</t>
-  </si>
-  <si>
-    <t>Le numéro du brevet étranger / national est le numéro de la demande déposée antérieurement.
-Ex: 60/508,112</t>
-  </si>
-  <si>
-    <t>Priority Claim Kind Code</t>
-  </si>
-  <si>
-    <t>Code de type de revendications de priorité</t>
-  </si>
-  <si>
-    <t>Priority Claim Kind Code indicates if the previously filed application was filed in Canada or not.
-Ex: INTERNATIONAL, NATIONAL</t>
-  </si>
-  <si>
-    <t>Le code de type de revendications de priorité indique si la demande déposée antérieurement a été effectuée au Canada ou à l'étranger.
-Ex: INTERNATIONAL, NATIONAL</t>
-  </si>
-  <si>
-    <t>Priority Claim Country Code</t>
-  </si>
-  <si>
-    <t>Code du pays d'origine de revendications de priorité</t>
-  </si>
-  <si>
-    <t>Country code of the previously filed application
-Ex: CA, US
-Detail definition (STANDARD ST.3) can be found at:
-https://www.wipo.int/export/sites/www/standards/en/pdf/03-03-01.pdf</t>
-  </si>
-  <si>
-    <t>Le code du pays d'origine d'une demande déposée antérieurement.
-Ex: CA, US
-La définition détaillée (STANDARD ST.3) peut être trouvée à l'adresse suivante:
-https://www.wipo.int/export/sites/www/standards/fr/pdf/03-03-01.pdf</t>
-  </si>
-  <si>
-    <t>Priority Claim Country</t>
-  </si>
-  <si>
-    <t>Pays d'origine de revendications de priorité</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Country of the the previously filed application
-Ex: Canada, United States of America </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le pays d'origine d'une demande déposée antérieurement
-Ex: Canada, United States of America </t>
-  </si>
-  <si>
-    <t>Priority Claim Calendar Dt</t>
-  </si>
-  <si>
-    <t>Date de revendications de priorité</t>
-  </si>
-  <si>
-    <t>Date of the the previously filed application
-YYYY-MM-DD
-Ex: 2017-02-17</t>
-  </si>
-  <si>
-    <t>La date de dépôt d'une demande antérieure
-AAAA-MM-JJ
-Ex: 2017-02-17</t>
   </si>
   <si>
     <t>Filling Date</t>
@@ -1369,8 +1350,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1388,6 +1370,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1431,21 +1419,6 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1456,7 +1429,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFffffff"/>
       </patternFill>
     </fill>
   </fills>
@@ -1477,16 +1450,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1529,95 +1502,101 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="29">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="8" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="9" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1628,10 +1607,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1669,71 +1648,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1761,7 +1740,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1784,11 +1763,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1797,13 +1776,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1813,7 +1792,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1822,7 +1801,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1831,7 +1810,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1839,10 +1818,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1907,7 +1886,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1917,233 +1896,279 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="85.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="99.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="10" width="46.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="52.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="17" width="85.14785714285713" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="17" width="99.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="B2" s="18"/>
-    </row>
-    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="24" t="s">
         <v>203</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="24" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="34.15" customFormat="1" s="1">
+      <c r="A4" s="25" t="s">
         <v>205</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="25" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="B6" s="19"/>
-    </row>
-    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="B6" s="26"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="24" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A8" s="25" t="s">
         <v>210</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="25" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A9" s="25" t="s">
         <v>212</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="25" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A10" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="25" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A12" s="27" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="24" t="s">
         <v>217</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="24" t="s">
         <v>218</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="24" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="28" t="s">
         <v>221</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="28" t="s">
         <v>223</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="28" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="28" t="s">
         <v>225</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="D15" s="28" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="A16" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="28" t="s">
         <v>229</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="D16" s="28" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+      <c r="A17" s="28" t="s">
         <v>231</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D17" s="28" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+      <c r="A18" s="28" t="s">
         <v>234</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="28" t="s">
         <v>235</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="28" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="A19" s="28" t="s">
         <v>237</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C19" s="28" t="s">
         <v>238</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="28" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+      <c r="A20" s="28" t="s">
         <v>240</v>
       </c>
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="28" t="s">
         <v>241</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="28" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+      <c r="A22" s="23" t="s">
         <v>243</v>
       </c>
-      <c r="B22" s="18"/>
-    </row>
-    <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+      <c r="B22" s="23"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+      <c r="A23" s="24" t="s">
         <v>244</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="24" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+      <c r="A24" s="28" t="s">
         <v>246</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="25" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="16" t="s">
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+      <c r="A25" s="28" t="s">
         <v>248</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="28" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+      <c r="A26" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="28" t="s">
         <v>251</v>
       </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2156,7 +2181,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2166,12 +2191,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2179,293 +2206,291 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="47.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="176.5703125" style="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="25"/>
+    <col min="1" max="1" style="16" width="25.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="16" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="16" width="176.57642857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="21" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="47.25" customFormat="1" s="1">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="21" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="47.25" customFormat="1" s="1">
+      <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="21" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="47.25" customFormat="1" s="1">
+      <c r="A3" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="7" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="21" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="47.25" customFormat="1" s="1">
+      <c r="A4" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="7" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="21" customFormat="1" ht="330" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A5" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="22" t="s">
+      <c r="B5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="21" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="47.25" customFormat="1" s="1">
+      <c r="A6" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="22" t="s">
+      <c r="B6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="21" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="47.25" customFormat="1" s="1">
+      <c r="A7" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="B7" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="21" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="47.25" customFormat="1" s="1">
+      <c r="A8" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="B8" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="22" t="s">
+      <c r="B8" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A9" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="7" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A10" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="B10" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="22" t="s">
+      <c r="B10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="21" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A11" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="B11" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="22" t="s">
+      <c r="B11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A12" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="7" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A13" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="B13" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="22" t="s">
+      <c r="B13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="21" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="47.25" customFormat="1" s="1">
+      <c r="A14" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B14" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="22" t="s">
+      <c r="B14" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="21" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="47.25" customFormat="1" s="1">
+      <c r="A15" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="7" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="16" spans="1:3" s="21" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A16" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="B16" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="22" t="s">
+      <c r="B16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="21" customFormat="1" ht="150" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A17" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="B17" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="22" t="s">
+      <c r="B17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A18" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="7" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A19" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="7" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A20" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="7" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A21" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="7" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="21" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A22" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="B22" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="22" t="s">
+      <c r="B22" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="21" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A23" s="20" t="s">
         <v>199</v>
       </c>
-      <c r="B23" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="22" t="s">
+      <c r="B23" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="21" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A24" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="B24" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="22" t="s">
+      <c r="B24" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="21" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="47.25" customFormat="1" s="1">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2473,242 +2498,241 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="11" width="25.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="16" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="16" width="52.14785714285715" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="60" customFormat="1" s="1">
+      <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="22" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="22" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="B7" s="22" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A3" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="33" customFormat="1" s="1">
+      <c r="A4" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="87" customFormat="1" s="1">
+      <c r="A5" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A6" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="60" customFormat="1" s="1">
+      <c r="A7" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="22" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="B8" s="22" t="s">
+      <c r="C7" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="60" customFormat="1" s="1">
+      <c r="A8" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="22" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="B9" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" s="2" customFormat="1" ht="255" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="2" customFormat="1" ht="255" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="2" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>139</v>
+      <c r="C8" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A9" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="46.5" customFormat="1" s="1">
+      <c r="A10" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="46.5" customFormat="1" s="1">
+      <c r="A11" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="46.5" customFormat="1" s="1">
+      <c r="A12" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="46.5" customFormat="1" s="1">
+      <c r="A13" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="46.5" customFormat="1" s="1">
+      <c r="A14" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A15" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="235.5" customFormat="1" s="1">
+      <c r="A16" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A17" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A18" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="114" customFormat="1" s="1">
+      <c r="A19" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A20" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -2717,205 +2741,207 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C35" sqref="C34:C35"/>
+      <pane state="frozen" activePane="bottomLeft" topLeftCell="A3" ySplit="2" xSplit="0"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="51.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="10" width="28.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="28.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="16" width="33.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="17" width="15.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="17" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="16" width="51.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="16" width="51.29071428571429" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="73.5">
+      <c r="A3" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="str">
-        <f t="shared" ref="C3:C8" si="0">A3 &amp;  " - " &amp; B3</f>
-        <v>Patent Number - Numéro du brevet</v>
-      </c>
-      <c r="D3" s="9" t="s">
+      <c r="C3" s="6">
+        <f>A3 &amp;  " - " &amp; B3</f>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="C4" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Foreign Application/Patent Number - Numéro du brevet étranger / national</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="46.5">
+      <c r="A4" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="6">
+        <f>A4 &amp;  " - " &amp; B4</f>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Priority Claim Kind Code - Code de type de revendications de priorité</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="F4" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="60">
+      <c r="A5" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="6">
+        <f>A5 &amp;  " - " &amp; B5</f>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="C6" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Priority Claim Country Code - Code du pays d'origine de revendications de priorité</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="F5" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="100.5">
+      <c r="A6" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="6">
+        <f>A6 &amp;  " - " &amp; B6</f>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="C7" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Priority Claim Country - Pays d'origine de revendications de priorité</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="F6" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="46.5">
+      <c r="A7" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="6">
+        <f>A7 &amp;  " - " &amp; B7</f>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="C8" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Priority Claim Calendar Dt - Date de revendications de priorité</v>
-      </c>
-      <c r="D8" s="9" t="s">
+      <c r="F7" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="46.5">
+      <c r="A8" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="6">
+        <f>A8 &amp;  " - " &amp; B8</f>
+      </c>
+      <c r="D8" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="F8" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2923,172 +2949,173 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane state="frozen" activePane="bottomLeft" topLeftCell="A3" ySplit="2" xSplit="0"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="61.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="59.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="10" width="32.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="27.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="16" width="31.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="17.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="17.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="61.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="10" width="59.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="7" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="16.9" customFormat="1" s="1">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="str">
+      <c r="C3" s="6">
         <f>A3 &amp;  " - " &amp; B3</f>
-        <v>Patent Number  - Numéro du brevet</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      </c>
+      <c r="D3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="3" t="str">
+      <c r="C4" s="6">
         <f>A4 &amp;  " - " &amp; B4</f>
-        <v>Language of Filing Code - Langue du type de dépôt</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="3" t="str">
+      <c r="C5" s="6">
         <f>A5 &amp;  " - " &amp; B5</f>
-        <v>Abstract Language Code - Code de la langue du résumé</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="3" t="str">
+      <c r="C6" s="6">
         <f>A6 &amp;  " - " &amp; B6</f>
-        <v>Abstract Text - Texte de l’abrégé</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="15" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="3" t="str">
+      <c r="C7" s="6">
         <f>A7 &amp;  " - " &amp; B7</f>
-        <v xml:space="preserve">Abstract Text Sequence Number - Numéro de séquence du texte de l'abrégé </v>
-      </c>
-      <c r="D7" s="9" t="s">
+      </c>
+      <c r="D7" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="7" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3098,167 +3125,287 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane state="frozen" activePane="bottomLeft" topLeftCell="A3" ySplit="2" xSplit="0"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="17" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="17" width="19.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="32.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="17" width="17.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="17.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="17" width="43.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="17" width="43.29071428571429" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="12" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.45" customFormat="1" s="1">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="str">
+      <c r="C3" s="6">
         <f>A3 &amp;  " - " &amp; B3</f>
-        <v>Patent Number  - Numéro du brevet</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      </c>
+      <c r="D3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="3" t="str">
+      <c r="C4" s="6">
         <f>A4 &amp;  " - " &amp; B4</f>
-        <v>Language of Filing Code - Langue du type de dépôt</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="3" t="str">
+      <c r="C5" s="6">
         <f>A5 &amp;  " - " &amp; B5</f>
-        <v>Disclosure Text - Texte de la divulgation</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="15" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="C6" s="3" t="str">
+      <c r="C6" s="6">
         <f>A6 &amp;  " - " &amp; B6</f>
-        <v xml:space="preserve">Disclosure Text Sequence Number - Numéro de séquence du texte de la divulgation </v>
-      </c>
-      <c r="D6" s="9" t="s">
+      </c>
+      <c r="D6" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="5:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="5:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="5:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="5:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="5:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E21" s="5"/>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3266,156 +3413,180 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane state="frozen" activePane="bottomLeft" topLeftCell="A3" ySplit="2" xSplit="0"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="49.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="10" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="21.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="16" width="31.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="17.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="17.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="44.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="10" width="49.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="17" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="17" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="12" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-    </row>
-    <row r="3" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="str">
+      <c r="C3" s="6">
         <f>A3 &amp;  " - " &amp; B3</f>
-        <v>Patent Number  - Numéro du brevet</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      </c>
+      <c r="D3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="3" t="str">
+      <c r="C4" s="6">
         <f>A4 &amp;  " - " &amp; B4</f>
-        <v>Language of Filing Code - Langue du type de dépôt</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="7" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="3" t="str">
+      <c r="C5" s="6">
         <f>A5 &amp;  " - " &amp; B5</f>
-        <v>Claims Text - Texte des revendications</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="15" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="3" t="str">
+      <c r="C6" s="6">
         <f>A6 &amp;  " - " &amp; B6</f>
-        <v>Claim Text Sequence Number - Numéro de séquence du texte des revendications</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      </c>
+      <c r="D6" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="7" t="s">
         <v>85</v>
       </c>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3423,450 +3594,459 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane state="frozen" activePane="bottomLeft" topLeftCell="A3" ySplit="2" xSplit="0"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="10" width="33.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="42.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="39.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="11" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="11" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="36.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="36.29071428571429" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="str">
-        <f t="shared" ref="C3:C18" si="0">A3 &amp;  " - " &amp; B3</f>
-        <v>Patent Number - Numéro du brevet</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="C3" s="6">
+        <f>A3 &amp;  " - " &amp; B3</f>
+      </c>
+      <c r="D3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>IPC Classification Sequence Number - Numéro de séquence de la classification de la CIB</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="6">
+        <f>A4 &amp;  " - " &amp; B4</f>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>IPC Version Date - Date de la version de la CIB</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="C5" s="6">
+        <f>A5 &amp;  " - " &amp; B5</f>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A6" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Classification Level - Niveau de classification</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="C6" s="6">
+        <f>A6 &amp;  " - " &amp; B6</f>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Classification Status Code - Code du statut de classification</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="C7" s="6">
+        <f>A7 &amp;  " - " &amp; B7</f>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>Classfication Status - Statut de classification</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="C8" s="6">
+        <f>A8 &amp;  " - " &amp; B8</f>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="7" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>IPC Section Code - Code de la section de la CIB</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="C9" s="6">
+        <f>A9 &amp;  " - " &amp; B9</f>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>IPC Section - Section de la CIB</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="C10" s="6">
+        <f>A10 &amp;  " - " &amp; B10</f>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>IPC Class Code - Code de la classe de la CIB</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="C11" s="6">
+        <f>A11 &amp;  " - " &amp; B11</f>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A12" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>IPC Class - Classe de la CIB</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="2" t="s">
+      <c r="C12" s="6">
+        <f>A12 &amp;  " - " &amp; B12</f>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A13" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>IPC Subclass Code - Code de la sous-classe de la CIB</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="C13" s="6">
+        <f>A13 &amp;  " - " &amp; B13</f>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A14" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>IPC Subclass - Sous-classe de la CIB</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="C14" s="6">
+        <f>A14 &amp;  " - " &amp; B14</f>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="7" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A15" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>IPC Main Group Code - Code du groupe principal de la CIB</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="C15" s="6">
+        <f>A15 &amp;  " - " &amp; B15</f>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A16" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>IPC Group - Groupe de la CIB</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="C16" s="6">
+        <f>A16 &amp;  " - " &amp; B16</f>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A17" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>IPC Subgroup Code - Code du sous-groupe de la CIB</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="C17" s="6">
+        <f>A17 &amp;  " - " &amp; B17</f>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A18" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>IPC Subgroup - Sous-groupe de la CIB</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="2" t="s">
+      <c r="C18" s="6">
+        <f>A18 &amp;  " - " &amp; B18</f>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="A19" s="8"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+      <c r="A20" s="8" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+      <c r="A21" s="9" t="s">
         <v>71</v>
       </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>